<commit_message>
CDV_AC curve data modified
</commit_message>
<xml_diff>
--- a/Files/Airfield_AC_Curve.xlsx
+++ b/Files/Airfield_AC_Curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VS_PCI\PCI\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1053C37-E943-439F-9348-363268D1D2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FD8C8A-3261-4119-9090-98A98480FCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="11">
   <si>
     <t>Density</t>
   </si>
@@ -75,18 +75,6 @@
   </si>
   <si>
     <t>q6</t>
-  </si>
-  <si>
-    <t>q7</t>
-  </si>
-  <si>
-    <t>q8</t>
-  </si>
-  <si>
-    <t>q9</t>
-  </si>
-  <si>
-    <t>q10</t>
   </si>
 </sst>
 </file>
@@ -6109,15 +6097,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E7E021-2638-47D1-B5DF-2338E308BB89}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
@@ -6139,20 +6127,8 @@
       <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -6169,25 +6145,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="6">
-        <v>1000</v>
-      </c>
-      <c r="I2" s="6">
-        <v>1000</v>
-      </c>
-      <c r="J2" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>10</v>
       </c>
@@ -6204,25 +6168,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="6">
-        <v>1001</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
       </c>
-      <c r="H3" s="6">
-        <v>1001</v>
-      </c>
-      <c r="I3" s="6">
-        <v>1001</v>
-      </c>
-      <c r="J3" s="6">
-        <v>1001</v>
-      </c>
-      <c r="K3" s="6">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>20</v>
       </c>
@@ -6239,25 +6191,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="6">
-        <v>1002</v>
+        <v>0</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
       </c>
-      <c r="H4" s="6">
-        <v>1002</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1002</v>
-      </c>
-      <c r="J4" s="6">
-        <v>1002</v>
-      </c>
-      <c r="K4" s="6">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>30</v>
       </c>
@@ -6274,25 +6214,13 @@
         <v>8</v>
       </c>
       <c r="F5" s="6">
-        <v>1003</v>
+        <v>8</v>
       </c>
       <c r="G5" s="6">
         <v>8</v>
       </c>
-      <c r="H5" s="6">
-        <v>1003</v>
-      </c>
-      <c r="I5" s="6">
-        <v>1003</v>
-      </c>
-      <c r="J5" s="6">
-        <v>1003</v>
-      </c>
-      <c r="K5" s="6">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>40</v>
       </c>
@@ -6309,25 +6237,13 @@
         <v>15</v>
       </c>
       <c r="F6" s="6">
-        <v>1004</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6">
         <v>15</v>
       </c>
-      <c r="H6" s="6">
-        <v>1004</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1004</v>
-      </c>
-      <c r="J6" s="6">
-        <v>1004</v>
-      </c>
-      <c r="K6" s="6">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>50</v>
       </c>
@@ -6344,25 +6260,13 @@
         <v>22.8</v>
       </c>
       <c r="F7" s="6">
-        <v>1005</v>
+        <v>22.8</v>
       </c>
       <c r="G7" s="6">
         <v>22.8</v>
       </c>
-      <c r="H7" s="6">
-        <v>1005</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1005</v>
-      </c>
-      <c r="J7" s="6">
-        <v>1005</v>
-      </c>
-      <c r="K7" s="6">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>60</v>
       </c>
@@ -6379,25 +6283,13 @@
         <v>29.2</v>
       </c>
       <c r="F8" s="6">
-        <v>1006</v>
+        <v>29.2</v>
       </c>
       <c r="G8" s="6">
         <v>29.2</v>
       </c>
-      <c r="H8" s="6">
-        <v>1006</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1006</v>
-      </c>
-      <c r="J8" s="6">
-        <v>1006</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>70</v>
       </c>
@@ -6414,25 +6306,13 @@
         <v>35.9</v>
       </c>
       <c r="F9" s="6">
-        <v>1007</v>
+        <v>35.9</v>
       </c>
       <c r="G9" s="6">
         <v>35.9</v>
       </c>
-      <c r="H9" s="6">
-        <v>1007</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1007</v>
-      </c>
-      <c r="J9" s="6">
-        <v>1007</v>
-      </c>
-      <c r="K9" s="6">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>80</v>
       </c>
@@ -6449,25 +6329,13 @@
         <v>41.5</v>
       </c>
       <c r="F10" s="6">
-        <v>1008</v>
+        <v>41.5</v>
       </c>
       <c r="G10" s="6">
         <v>41.5</v>
       </c>
-      <c r="H10" s="6">
-        <v>1008</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1008</v>
-      </c>
-      <c r="J10" s="6">
-        <v>1008</v>
-      </c>
-      <c r="K10" s="6">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>90</v>
       </c>
@@ -6484,25 +6352,13 @@
         <v>47</v>
       </c>
       <c r="F11" s="6">
-        <v>1009</v>
+        <v>47</v>
       </c>
       <c r="G11" s="6">
         <v>47</v>
       </c>
-      <c r="H11" s="6">
-        <v>1009</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1009</v>
-      </c>
-      <c r="J11" s="6">
-        <v>1009</v>
-      </c>
-      <c r="K11" s="6">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>100</v>
       </c>
@@ -6519,25 +6375,13 @@
         <v>53</v>
       </c>
       <c r="F12" s="6">
-        <v>1010</v>
+        <v>53</v>
       </c>
       <c r="G12" s="6">
         <v>52</v>
       </c>
-      <c r="H12" s="6">
-        <v>1010</v>
-      </c>
-      <c r="I12" s="6">
-        <v>1010</v>
-      </c>
-      <c r="J12" s="6">
-        <v>1010</v>
-      </c>
-      <c r="K12" s="6">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>110</v>
       </c>
@@ -6554,25 +6398,13 @@
         <v>58</v>
       </c>
       <c r="F13" s="6">
-        <v>1011</v>
+        <v>57</v>
       </c>
       <c r="G13" s="6">
         <v>57</v>
       </c>
-      <c r="H13" s="6">
-        <v>1011</v>
-      </c>
-      <c r="I13" s="6">
-        <v>1011</v>
-      </c>
-      <c r="J13" s="6">
-        <v>1011</v>
-      </c>
-      <c r="K13" s="6">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>120</v>
       </c>
@@ -6589,25 +6421,13 @@
         <v>62.5</v>
       </c>
       <c r="F14" s="6">
-        <v>1012</v>
+        <v>62</v>
       </c>
       <c r="G14" s="6">
         <v>60.5</v>
       </c>
-      <c r="H14" s="6">
-        <v>1012</v>
-      </c>
-      <c r="I14" s="6">
-        <v>1012</v>
-      </c>
-      <c r="J14" s="6">
-        <v>1012</v>
-      </c>
-      <c r="K14" s="6">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>130</v>
       </c>
@@ -6624,25 +6444,13 @@
         <v>67</v>
       </c>
       <c r="F15" s="6">
-        <v>1013</v>
+        <v>66</v>
       </c>
       <c r="G15" s="6">
         <v>64.400000000000006</v>
       </c>
-      <c r="H15" s="6">
-        <v>1013</v>
-      </c>
-      <c r="I15" s="6">
-        <v>1013</v>
-      </c>
-      <c r="J15" s="6">
-        <v>1013</v>
-      </c>
-      <c r="K15" s="6">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>140</v>
       </c>
@@ -6659,25 +6467,13 @@
         <v>71.5</v>
       </c>
       <c r="F16" s="6">
-        <v>1014</v>
+        <v>70</v>
       </c>
       <c r="G16" s="6">
         <v>67.8</v>
       </c>
-      <c r="H16" s="6">
-        <v>1014</v>
-      </c>
-      <c r="I16" s="6">
-        <v>1014</v>
-      </c>
-      <c r="J16" s="6">
-        <v>1014</v>
-      </c>
-      <c r="K16" s="6">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>150</v>
       </c>
@@ -6694,25 +6490,13 @@
         <v>75.5</v>
       </c>
       <c r="F17" s="6">
-        <v>1015</v>
+        <v>74</v>
       </c>
       <c r="G17" s="6">
         <v>70.8</v>
       </c>
-      <c r="H17" s="6">
-        <v>1015</v>
-      </c>
-      <c r="I17" s="6">
-        <v>1015</v>
-      </c>
-      <c r="J17" s="6">
-        <v>1015</v>
-      </c>
-      <c r="K17" s="6">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>160</v>
       </c>
@@ -6729,25 +6513,13 @@
         <v>79</v>
       </c>
       <c r="F18" s="6">
-        <v>1016</v>
+        <v>77</v>
       </c>
       <c r="G18" s="6">
         <v>74</v>
       </c>
-      <c r="H18" s="6">
-        <v>1016</v>
-      </c>
-      <c r="I18" s="6">
-        <v>1016</v>
-      </c>
-      <c r="J18" s="6">
-        <v>1016</v>
-      </c>
-      <c r="K18" s="6">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>170</v>
       </c>
@@ -6764,25 +6536,13 @@
         <v>82.1</v>
       </c>
       <c r="F19" s="6">
-        <v>1017</v>
+        <v>80</v>
       </c>
       <c r="G19" s="6">
         <v>76.8</v>
       </c>
-      <c r="H19" s="6">
-        <v>1017</v>
-      </c>
-      <c r="I19" s="6">
-        <v>1017</v>
-      </c>
-      <c r="J19" s="6">
-        <v>1017</v>
-      </c>
-      <c r="K19" s="6">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>180</v>
       </c>
@@ -6799,22 +6559,10 @@
         <v>85</v>
       </c>
       <c r="F20" s="6">
-        <v>1018</v>
+        <v>82</v>
       </c>
       <c r="G20" s="6">
         <v>79</v>
-      </c>
-      <c r="H20" s="6">
-        <v>1018</v>
-      </c>
-      <c r="I20" s="6">
-        <v>1018</v>
-      </c>
-      <c r="J20" s="6">
-        <v>1018</v>
-      </c>
-      <c r="K20" s="6">
-        <v>1018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>